<commit_message>
Added the new concert 'Plug & Play Jam Session (Apr 6, 2023)'
</commit_message>
<xml_diff>
--- a/Development/Shiny/data/Dead Dogs Live Concerts.xlsx
+++ b/Development/Shiny/data/Dead Dogs Live Concerts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PC3\Operation Ultra\09 - R\18 - Blog &amp; Projects\RShiny\Apps\Dead Dogs Analytics\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PC3\Operation Ultra\09 - R\Projects\Dead Dogs Analytics\Dead Dogs Analytics ShinyApp\Production\Shiny\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC945800-2D76-44FC-BCE5-9E71488A7D0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D72283-73A2-4DDD-8D60-0F9313AFA0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
   <si>
     <t>Id</t>
   </si>
@@ -287,6 +287,21 @@
   </si>
   <si>
     <t>Barona Beer Festival</t>
+  </si>
+  <si>
+    <t>Melegnano (MI)</t>
+  </si>
+  <si>
+    <t>Musicolepsia</t>
+  </si>
+  <si>
+    <t>Plug &amp; Play Jam Session (Apr 6, 2023)</t>
+  </si>
+  <si>
+    <t>06/04/2023</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="300" height="169" src="https://www.youtube.com/embed/playlist?list=PLhIw1_0YGPEStVIUkVyv2ZB4PlUeK02QW"&gt;&lt;/iframe&gt;</t>
   </si>
 </sst>
 </file>
@@ -335,10 +350,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,23 +633,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="129.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="129.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -661,7 +675,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -684,7 +698,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -707,7 +721,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -733,7 +747,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -759,7 +773,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -785,7 +799,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -811,7 +825,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -837,7 +851,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -863,7 +877,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -889,7 +903,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -915,7 +929,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -937,11 +951,11 @@
       <c r="G12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -963,11 +977,11 @@
       <c r="G13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -990,7 +1004,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -1011,6 +1025,32 @@
       </c>
       <c r="G15" s="1" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16">
+        <v>45.357970954483299</v>
+      </c>
+      <c r="E16">
+        <v>9.3146710101658599</v>
+      </c>
+      <c r="F16">
+        <v>2023</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1028,34 +1068,34 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="17" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>

</xml_diff>